<commit_message>
Atualização no script de automação
</commit_message>
<xml_diff>
--- a/Comprovantes/comprovantes_funcionario.xlsx
+++ b/Comprovantes/comprovantes_funcionario.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,8 +421,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="40" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
@@ -458,106 +458,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mateus Esteves:</t>
+          <t>Você</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19:19, 25/03/2025</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 23,67</t>
+          <t>R$ 200,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SHIBATA COMERCIO E ATACADO DE PROD...</t>
+          <t>COMERCIO DE POLPAS SOUZA E DIAS LTD...</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>Funcionário</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Mateus Esteves:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>19:21, 25/03/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>R$ 24,00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Gabriel Willian da Costa Souza</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Funcionário</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Você</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Desconhecido</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>R$ 200,00</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>COMERCIO DE POLPAS SOUZA E DIAS LTD...</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Funcionário</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Mateus Esteves:</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>20:36, 25/03/2025</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>R$ 67,45</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>SHIBATA COMERCIO E ATACADO DE PROD...</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
         <is>
           <t>Funcionário</t>
         </is>

</xml_diff>